<commit_message>
Name & Matrikelnummer hinzugefügt
</commit_message>
<xml_diff>
--- a/Ausarbeitung_Kapitelzuordnung.xlsx
+++ b/Ausarbeitung_Kapitelzuordnung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dokumente\FH_Dortmund\Master\Anwendungen_MI\schriftlicher_Teil\tex\Ausarbeitung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TobyV2\Documents\AMiAusarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -233,16 +233,16 @@
     <t>Dominique Latza</t>
   </si>
   <si>
-    <t>Andy</t>
-  </si>
-  <si>
     <t>Alle</t>
   </si>
   <si>
     <t>Matrikel Nummer</t>
   </si>
   <si>
-    <t>Tobias</t>
+    <t>Tobias Rempel</t>
+  </si>
+  <si>
+    <t>Andy Kruder</t>
   </si>
 </sst>
 </file>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,160 +1064,194 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C29" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C30" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C32" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C33" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C34" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C35" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C36" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C37" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C38" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C39" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C40" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C41" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C42" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C43" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C44" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C45" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C46" s="5"/>
     </row>
@@ -1226,7 +1260,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C47" s="5"/>
     </row>
@@ -1235,7 +1269,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C48" s="5"/>
     </row>
@@ -1244,7 +1278,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C49" s="5"/>
     </row>
@@ -1275,7 +1309,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C52" s="5"/>
     </row>
@@ -1284,7 +1318,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C53" s="5"/>
     </row>
@@ -1293,7 +1327,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C54" s="5"/>
     </row>
@@ -1430,7 +1464,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" s="8"/>
     </row>

</xml_diff>

<commit_message>
Kapitel 5&6 getauscht, Zuordnungsdokument angepasst
</commit_message>
<xml_diff>
--- a/Ausarbeitung_Kapitelzuordnung.xlsx
+++ b/Ausarbeitung_Kapitelzuordnung.xlsx
@@ -110,69 +110,6 @@
     <t xml:space="preserve">4.2. Objektorientierter Entwurf </t>
   </si>
   <si>
-    <t xml:space="preserve">5. Bildakquise und Datenaufbereitung </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.1. Bildakquise </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.2. Kodierung </t>
-  </si>
-  <si>
-    <t>5.3. Dekodierung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4. Implementierung mit FFmpeg </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4.1. Auswahl eines Videocodecs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4.2. Nutzung des MediaCodec </t>
-  </si>
-  <si>
-    <t>5.4.3. Verarbeitung des Datenstroms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4.4. Konfiguration des MediaCodec </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4.5. Performance und Funktionalität </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5. Implementierung mit X11Lib und LZ4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.1. Bildakquise mit X11Lib </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.2. Datenreduktion </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.3. Kompression </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.4. Verarbeitung auf dem Smartphone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.5. Performance und Funktionalität </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.5.6. Optimierungspotenzial </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. SonoScape Analyse </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.1. System Struktur </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.2. Root Zugriff </t>
-  </si>
-  <si>
-    <t>6.3. Netzwerk Verbindung</t>
-  </si>
-  <si>
     <t>7. Bildverarbeitung</t>
   </si>
   <si>
@@ -243,6 +180,69 @@
   </si>
   <si>
     <t>Andy Kruder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. SonoScape Analyse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1. System Struktur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.2. Root Zugriff </t>
+  </si>
+  <si>
+    <t>5.3. Netzwerk Verbindung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Bildakquise und Datenaufbereitung </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1. Bildakquise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2. Kodierung </t>
+  </si>
+  <si>
+    <t>6.3. Dekodierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4. Implementierung mit FFmpeg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4.1. Auswahl eines Videocodecs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4.2. Nutzung des MediaCodec </t>
+  </si>
+  <si>
+    <t>6.4.3. Verarbeitung des Datenstroms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4.4. Konfiguration des MediaCodec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4.5. Performance und Funktionalität </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5. Implementierung mit X11Lib und LZ4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.1. Bildakquise mit X11Lib </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.2. Datenreduktion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.3. Kompression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.4. Verarbeitung auf dem Smartphone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.5. Performance und Funktionalität </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.6. Optimierungspotenzial </t>
   </si>
 </sst>
 </file>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5">
         <v>7080245</v>
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5">
         <v>7080245</v>
@@ -789,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5">
         <v>7080245</v>
@@ -800,7 +800,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5">
         <v>7080245</v>
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5">
         <v>7080245</v>
@@ -822,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5">
         <v>7080245</v>
@@ -833,7 +833,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5">
         <v>7080245</v>
@@ -844,7 +844,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C9" s="5">
         <v>7080245</v>
@@ -855,7 +855,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5">
         <v>7080245</v>
@@ -866,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C11" s="5">
         <v>7080245</v>
@@ -877,7 +877,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5">
         <v>7080245</v>
@@ -888,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5">
         <v>7080245</v>
@@ -899,7 +899,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C14" s="5">
         <v>7077438</v>
@@ -910,7 +910,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5">
         <v>7077438</v>
@@ -921,7 +921,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5">
         <v>7077438</v>
@@ -932,7 +932,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5">
         <v>7077438</v>
@@ -943,7 +943,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5">
         <v>7077438</v>
@@ -954,7 +954,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
         <v>7077438</v>
@@ -965,7 +965,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C20" s="5">
         <v>7077438</v>
@@ -976,7 +976,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5">
         <v>7077438</v>
@@ -987,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C22" s="5">
         <v>7077438</v>
@@ -998,7 +998,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C23" s="5">
         <v>7077438</v>
@@ -1009,7 +1009,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5">
         <v>7080245</v>
@@ -1020,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5">
         <v>7080245</v>
@@ -1031,7 +1031,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5">
         <v>7080245</v>
@@ -1042,7 +1042,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C27" s="5">
         <v>7080245</v>
@@ -1053,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C28" s="5">
         <v>7080245</v>
@@ -1061,54 +1061,46 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="5">
-        <v>7080879</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="5">
-        <v>7080879</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="5">
-        <v>7080879</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="5">
-        <v>7080879</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C33" s="5">
         <v>7080879</v>
@@ -1116,10 +1108,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C34" s="5">
         <v>7080879</v>
@@ -1127,10 +1119,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C35" s="5">
         <v>7080879</v>
@@ -1138,10 +1130,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C36" s="5">
         <v>7080879</v>
@@ -1149,10 +1141,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C37" s="5">
         <v>7080879</v>
@@ -1160,10 +1152,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C38" s="5">
         <v>7080879</v>
@@ -1171,10 +1163,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C39" s="5">
         <v>7080879</v>
@@ -1182,10 +1174,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C40" s="5">
         <v>7080879</v>
@@ -1193,10 +1185,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C41" s="5">
         <v>7080879</v>
@@ -1204,10 +1196,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C42" s="5">
         <v>7080879</v>
@@ -1215,10 +1207,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C43" s="5">
         <v>7080879</v>
@@ -1226,10 +1218,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C44" s="5">
         <v>7080879</v>
@@ -1237,10 +1229,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C45" s="5">
         <v>7080879</v>
@@ -1248,46 +1240,54 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C46" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C47" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C48" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C49" s="5">
+        <v>7080879</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C50" s="5">
         <v>7077438</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C51" s="5">
         <v>7080245</v>
@@ -1306,37 +1306,37 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C55" s="5">
         <v>7077438</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C56" s="5">
         <v>7077438</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C57" s="5">
         <v>7077438</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C58" s="5">
         <v>7077438</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C59" s="5">
         <v>7077438</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C60" s="5">
         <v>7077438</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C61" s="5">
         <v>7077438</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C62" s="5">
         <v>7077438</v>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C63" s="5">
         <v>7077438</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C64" s="5">
         <v>7077438</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C65" s="5">
         <v>7077438</v>
@@ -1454,17 +1454,17 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C67" s="8"/>
     </row>

</xml_diff>

<commit_message>
Titel hinzugefügt, Quelle auf Seite 1 gefixt
</commit_message>
<xml_diff>
--- a/Ausarbeitung_Kapitelzuordnung.xlsx
+++ b/Ausarbeitung_Kapitelzuordnung.xlsx
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1066,9 @@
       <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -1075,7 +1077,9 @@
       <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -1084,7 +1088,9 @@
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -1093,7 +1099,9 @@
       <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -1311,7 +1319,9 @@
       <c r="B52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="5"/>
+      <c r="C52" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -1320,7 +1330,9 @@
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -1329,7 +1341,9 @@
       <c r="B54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="5"/>
+      <c r="C54" s="5">
+        <v>7084984</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">

</xml_diff>